<commit_message>
Add more actions: [startTesting], [endTesting]
</commit_message>
<xml_diff>
--- a/inputdata/Automation Testcases.xlsx
+++ b/inputdata/Automation Testcases.xlsx
@@ -4,21 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="2955" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21180" windowHeight="10635" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
     <sheet name="Guideline" sheetId="5" r:id="rId2"/>
     <sheet name="Config" sheetId="4" r:id="rId3"/>
     <sheet name="LOGIN" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
-    <sheet name="PRESENTATION" sheetId="2" r:id="rId6"/>
+    <sheet name="PRESENTATION" sheetId="2" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">LOGIN!$A$9:$S$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">LOGIN!$A$9:$S$32</definedName>
     <definedName name="TC_BE_006">'[1]Back-End'!#REF!</definedName>
     <definedName name="TC_BE_020">'[1]Back-End'!#REF!</definedName>
   </definedNames>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="203">
   <si>
     <t>ID</t>
   </si>
@@ -233,12 +232,6 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>assertText</t>
-  </si>
-  <si>
-    <t>assertTitle</t>
-  </si>
-  <si>
     <t>back</t>
   </si>
   <si>
@@ -264,9 +257,6 @@
   </si>
   <si>
     <t>selectByText</t>
-  </si>
-  <si>
-    <t>selectByValue</t>
   </si>
   <si>
     <t>verifyDropdownSelectedText</t>
@@ -477,9 +467,6 @@
     <t>Click on [Browser] button to upload image</t>
   </si>
   <si>
-    <t>selectImage</t>
-  </si>
-  <si>
     <t>Wait for uploading</t>
   </si>
   <si>
@@ -506,15 +493,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>PASSED</t>
-  </si>
-  <si>
-    <t>Assert between text values</t>
-  </si>
-  <si>
-    <t>Assert page title</t>
-  </si>
-  <si>
     <t>Back to previous page. Like clicking on [Back] button on browser task bar</t>
   </si>
   <si>
@@ -602,31 +580,13 @@
     <t>SUNNY.png</t>
   </si>
   <si>
-    <t>Open page</t>
-  </si>
-  <si>
     <t>verifyListValue</t>
-  </si>
-  <si>
-    <t>Get list</t>
-  </si>
-  <si>
-    <t>http://www.vietjetair.com/Sites/Web/vi-VN/Home</t>
-  </si>
-  <si>
-    <t>id=ctl00_UcHeaderV31_DrLang</t>
-  </si>
-  <si>
-    <t>Quit</t>
   </si>
   <si>
     <t>Verify if returned values list are matched with expectation. 
 If expected list is more than 1 element, Addd '@' char before the second element and elements are separated by comma (Ex: Jan,@Feb,@Mar,@Apr)</t>
   </si>
   <si>
-    <t>Tiếng Việt,@English,@ภาษาไทย,@한국어 (o),@简体中文,@繁體中文</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
@@ -657,7 +617,43 @@
     <t>Clear cookies by name</t>
   </si>
   <si>
+    <t>storeText</t>
+  </si>
+  <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>Store [Presenation List] page title</t>
+  </si>
+  <si>
+    <t>{btnSubmit}</t>
+  </si>
+  <si>
+    <t>storeVal</t>
+  </si>
+  <si>
+    <t>selectByVal</t>
+  </si>
+  <si>
+    <t>get user name value</t>
+  </si>
+  <si>
+    <t>{username}</t>
+  </si>
+  <si>
+    <t>http://localhost:9080/cms/</t>
+  </si>
+  <si>
+    <t>endTesting</t>
+  </si>
+  <si>
+    <t>startTesting</t>
+  </si>
+  <si>
+    <t>Start test</t>
+  </si>
+  <si>
+    <t>selectFile</t>
   </si>
 </sst>
 </file>
@@ -1673,10 +1669,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1691,7 +1687,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="32" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="31" t="s">
@@ -1721,10 +1717,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>62</v>
@@ -1736,15 +1732,15 @@
         <v>68</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1752,23 +1748,23 @@
         <v>69</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>156</v>
+      <c r="E5" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1776,11 +1772,11 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>157</v>
+      <c r="E6" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1788,11 +1784,11 @@
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>200</v>
+      <c r="E7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1800,11 +1796,11 @@
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>202</v>
+      <c r="E8" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1813,10 +1809,10 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1825,11 +1821,9 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>159</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="4"/>
@@ -1837,10 +1831,10 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1849,10 +1843,10 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1861,10 +1855,10 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1873,10 +1867,10 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1885,10 +1879,10 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1897,10 +1891,10 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1909,10 +1903,10 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1921,10 +1915,10 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1933,10 +1927,10 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1945,10 +1939,10 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>136</v>
+        <v>5</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1957,10 +1951,10 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1969,10 +1963,10 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1984,7 +1978,7 @@
         <v>75</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1993,10 +1987,10 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2005,10 +1999,10 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>78</v>
+        <v>195</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2017,10 +2011,10 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2029,11 +2023,9 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="4"/>
@@ -2041,11 +2033,9 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>176</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="4"/>
@@ -2053,11 +2043,9 @@
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>177</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="4"/>
@@ -2065,10 +2053,10 @@
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2077,22 +2065,22 @@
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="60">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>191</v>
+        <v>131</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2101,22 +2089,22 @@
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>133</v>
+        <v>77</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="60">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2125,10 +2113,10 @@
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2137,36 +2125,72 @@
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>135</v>
+        <v>52</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="B38" s="30"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
+      <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
     </row>
     <row r="40" spans="1:6">
+      <c r="A40" s="4"/>
       <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" s="30"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2195,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:XFD15"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11:L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -2281,24 +2305,24 @@
       <c r="F4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="21">
-        <f>COUNTIF($L$11:$L$594,"PASSED")/COUNTA($L$11:$L$594)</f>
-        <v>1</v>
+      <c r="G4" s="21" t="e">
+        <f>COUNTIF($L$11:$L$597,"PASSED")/COUNTA($L$11:$L$597)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="N4" s="21">
-        <f>COUNTIF($N$11:N$594,"Pass")</f>
+        <f>COUNTIF($N$11:N$596,"Pass")</f>
         <v>0</v>
       </c>
       <c r="O4" s="21">
-        <f>COUNTIF($O$11:O$594,"Pass")</f>
+        <f>COUNTIF($O$11:O$596,"Pass")</f>
         <v>0</v>
       </c>
       <c r="P4" s="21">
-        <f>COUNTIF($P$11:P$594,"Pass")</f>
+        <f>COUNTIF($P$11:P$596,"Pass")</f>
         <v>0</v>
       </c>
       <c r="Q4" s="21">
-        <f>COUNTIF($Q$11:Q$594,"Pass")</f>
+        <f>COUNTIF($Q$11:Q$596,"Pass")</f>
         <v>0</v>
       </c>
     </row>
@@ -2318,24 +2342,24 @@
       <c r="F5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="21">
-        <f>COUNTIF($L$11:$L$594,"FAILED")/COUNTA($L$11:$L$594)</f>
+      <c r="G5" s="21" t="e">
+        <f>COUNTIF($L$11:$L$597,"FAILED")/COUNTA($L$11:$L$597)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N5" s="21">
+        <f>COUNTIF($N$11:N$596,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="N5" s="21">
-        <f>COUNTIF($N$11:N$594,"Fail")</f>
+      <c r="O5" s="21">
+        <f>COUNTIF($O$11:$O$596,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="O5" s="21">
-        <f>COUNTIF($O$11:$O$594,"Fail")</f>
+      <c r="P5" s="21">
+        <f>COUNTIF($P$11:$P$596,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="P5" s="21">
-        <f>COUNTIF($P$11:$P$594,"Fail")</f>
-        <v>0</v>
-      </c>
       <c r="Q5" s="21">
-        <f>COUNTIF($Q$11:$Q$594,"Fail")</f>
+        <f>COUNTIF($Q$11:$Q$596,"Fail")</f>
         <v>0</v>
       </c>
     </row>
@@ -2347,30 +2371,30 @@
         <v>21</v>
       </c>
       <c r="D6" s="21">
-        <f>COUNTIF($G$11:$G$594,"Yes")/COUNTA($A$11:$A$594)</f>
+        <f>COUNTIF($G$11:$G$596,"Yes")/COUNTA($A$11:$A$596)</f>
         <v>0.75</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="21">
-        <f>COUNTIF($L$12:$L$594,"Not Test")/COUNTA($L$11:$L$594)</f>
+      <c r="G6" s="21" t="e">
+        <f>COUNTIF($L$12:$L$597,"Not Test")/COUNTA($L$11:$L$597)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="21">
+        <f>COUNTIF($N$11:N$596,"Not Test")</f>
         <v>0</v>
       </c>
-      <c r="N6" s="21">
-        <f>COUNTIF($N$11:N$594,"Not Test")</f>
+      <c r="O6" s="21">
+        <f>COUNTIF($H$11:$H$596,"Not Test")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="21">
-        <f>COUNTIF($H$11:$H$594,"Not Test")</f>
+      <c r="P6" s="21">
+        <f>COUNTIF($P$11:$P$596,"Not Test")</f>
         <v>0</v>
       </c>
-      <c r="P6" s="21">
-        <f>COUNTIF($P$11:$P$594,"Not Test")</f>
-        <v>0</v>
-      </c>
       <c r="Q6" s="21">
-        <f>COUNTIF($Q$11:$Q$594,"Not Test")</f>
+        <f>COUNTIF($Q$11:$Q$596,"Not Test")</f>
         <v>0</v>
       </c>
     </row>
@@ -2455,7 +2479,7 @@
     </row>
     <row r="10" spans="1:20" s="2" customFormat="1">
       <c r="A10" s="17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -2479,35 +2503,33 @@
     </row>
     <row r="11" spans="1:20" s="2" customFormat="1" ht="75">
       <c r="A11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="F11" s="22" t="s">
         <v>88</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>91</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" t="s">
-        <v>153</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="L11"/>
       <c r="M11" t="s">
         <v>7</v>
       </c>
@@ -2522,7 +2544,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>55</v>
@@ -2532,9 +2554,6 @@
       </c>
       <c r="K12" s="25" t="s">
         <v>56</v>
-      </c>
-      <c r="L12" t="s">
-        <v>153</v>
       </c>
       <c r="M12" t="s">
         <v>7</v>
@@ -2555,19 +2574,16 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
-        <v>85</v>
+        <v>196</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>55</v>
+        <v>194</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="L13" t="s">
-        <v>153</v>
+        <v>57</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>197</v>
       </c>
       <c r="M13" t="s">
         <v>7</v>
@@ -2588,17 +2604,16 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K14" s="4"/>
-      <c r="L14" t="s">
-        <v>153</v>
+        <v>58</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>80</v>
       </c>
       <c r="M14" t="s">
         <v>7</v>
@@ -2610,7 +2625,7 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="1:20" ht="30">
+    <row r="15" spans="1:20">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2619,20 +2634,15 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="L15" t="s">
-        <v>153</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="K15" s="4"/>
       <c r="M15" t="s">
         <v>7</v>
       </c>
@@ -2652,15 +2662,16 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>95</v>
+        <v>192</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" t="s">
-        <v>153</v>
+        <v>190</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="M16" t="s">
         <v>7</v>
@@ -2672,28 +2683,29 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:20" ht="60">
-      <c r="A17" s="2" t="s">
-        <v>96</v>
-      </c>
+    <row r="17" spans="1:20" ht="30">
+      <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>151</v>
-      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" t="s">
+        <v>7</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -2701,39 +2713,22 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" spans="1:20" ht="75">
-      <c r="A18" s="2" t="s">
-        <v>149</v>
-      </c>
+    <row r="18" spans="1:20">
+      <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>82</v>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="2"/>
-      <c r="L18" t="s">
-        <v>153</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
       <c r="M18" t="s">
         <v>7</v>
       </c>
@@ -2744,32 +2739,28 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:20" ht="60">
+      <c r="A19" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K19" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="L19" t="s">
-        <v>153</v>
-      </c>
-      <c r="M19" t="s">
-        <v>7</v>
-      </c>
+      <c r="F19" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -2777,29 +2768,36 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" spans="1:20">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:20" ht="75">
+      <c r="A20" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4" t="s">
-        <v>85</v>
+      <c r="C20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K20" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="L20" t="s">
-        <v>153</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K20" s="2"/>
       <c r="M20" t="s">
         <v>7</v>
       </c>
@@ -2819,17 +2817,16 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K21" s="4"/>
-      <c r="L21" t="s">
-        <v>153</v>
+        <v>57</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>101</v>
       </c>
       <c r="M21" t="s">
         <v>7</v>
@@ -2841,7 +2838,7 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
     </row>
-    <row r="22" spans="1:20" ht="30">
+    <row r="22" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2849,20 +2846,17 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="27" t="s">
-        <v>101</v>
+      <c r="H22" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K22" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="L22" t="s">
-        <v>153</v>
       </c>
       <c r="M22" t="s">
         <v>7</v>
@@ -2883,16 +2877,15 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="K23" s="4"/>
-      <c r="L23" t="s">
-        <v>153</v>
-      </c>
       <c r="M23" t="s">
         <v>7</v>
       </c>
@@ -2903,41 +2896,35 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" spans="1:20" s="2" customFormat="1" ht="60">
-      <c r="A24" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>82</v>
+    <row r="24" spans="1:20" ht="30">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L24" t="s">
-        <v>153</v>
+        <v>52</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>100</v>
       </c>
       <c r="M24" t="s">
         <v>7</v>
       </c>
-      <c r="T24" s="24"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="4"/>
@@ -2947,21 +2934,12 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="H25" s="27"/>
       <c r="I25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K25" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="L25" t="s">
-        <v>153</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
       <c r="M25" t="s">
         <v>7</v>
       </c>
@@ -2972,38 +2950,39 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4" t="s">
-        <v>85</v>
+    <row r="26" spans="1:20" s="2" customFormat="1" ht="60">
+      <c r="A26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K26" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="L26" t="s">
-        <v>153</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="L26"/>
       <c r="M26" t="s">
         <v>7</v>
       </c>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
+      <c r="T26" s="24"/>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="4"/>
@@ -3014,17 +2993,16 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K27" s="4"/>
-      <c r="L27" t="s">
-        <v>153</v>
+        <v>57</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>56</v>
       </c>
       <c r="M27" t="s">
         <v>7</v>
@@ -3045,16 +3023,16 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J28" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="L28" t="s">
-        <v>153</v>
+        <v>55</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K28" s="23" t="s">
+        <v>80</v>
       </c>
       <c r="M28" t="s">
         <v>7</v>
@@ -3066,7 +3044,7 @@
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" spans="1:20" ht="30">
+    <row r="29" spans="1:20">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -3075,20 +3053,15 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L29" t="s">
-        <v>153</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="K29" s="4"/>
       <c r="M29" t="s">
         <v>7</v>
       </c>
@@ -3108,15 +3081,13 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" t="s">
-        <v>153</v>
+        <v>59</v>
+      </c>
+      <c r="J30" s="26" t="s">
+        <v>108</v>
       </c>
       <c r="M30" t="s">
         <v>7</v>
@@ -3128,19 +3099,80 @@
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
     </row>
+    <row r="31" spans="1:20" ht="30">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M31" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="M32" t="s">
+        <v>7</v>
+      </c>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+    </row>
+    <row r="33" spans="13:13">
+      <c r="M33" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A9:S30"/>
+  <autoFilter ref="A9:S32"/>
   <mergeCells count="2">
     <mergeCell ref="G8:M8"/>
     <mergeCell ref="N8:Q8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J11" r:id="rId1"/>
-    <hyperlink ref="K13" r:id="rId2"/>
-    <hyperlink ref="J18" r:id="rId3"/>
-    <hyperlink ref="K20" r:id="rId4"/>
-    <hyperlink ref="J24" r:id="rId5"/>
-    <hyperlink ref="K26" r:id="rId6"/>
+    <hyperlink ref="K14" r:id="rId2"/>
+    <hyperlink ref="J20" r:id="rId3"/>
+    <hyperlink ref="K22" r:id="rId4"/>
+    <hyperlink ref="J26" r:id="rId5"/>
+    <hyperlink ref="K28" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -3149,9 +3181,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Config!$E$3:$E$185</xm:f>
+            <xm:f>Config!$E$3:$E$187</xm:f>
           </x14:formula1>
-          <xm:sqref>I11:I30</xm:sqref>
+          <xm:sqref>I11:I32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3161,21 +3193,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="G18" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="8" max="8" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.85546875" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="8" max="8" width="28.5703125" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="9" max="9" width="25.42578125" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="10" max="10" width="25.7109375" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="11" max="11" width="19.42578125" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="12" max="12" width="14.85546875" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="13" max="13" width="13.5703125" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="14" max="14" width="13.28515625" style="2" customWidth="1"/>
+    <col min="15" max="17" width="13.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="20" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="18" customFormat="1">
+    <row r="1" spans="1:19" s="18" customFormat="1">
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -3184,7 +3229,7 @@
       <c r="L1" s="2"/>
       <c r="R1" s="20"/>
     </row>
-    <row r="2" spans="1:20" s="18" customFormat="1">
+    <row r="2" spans="1:19" s="18" customFormat="1">
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -3193,7 +3238,7 @@
       <c r="L2" s="2"/>
       <c r="R2" s="20"/>
     </row>
-    <row r="3" spans="1:20" s="2" customFormat="1" ht="30">
+    <row r="3" spans="1:19">
       <c r="A3" s="16" t="s">
         <v>15</v>
       </c>
@@ -3222,7 +3267,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="2" customFormat="1" ht="30">
+    <row r="4" spans="1:19">
       <c r="A4" s="16" t="s">
         <v>24</v>
       </c>
@@ -3239,27 +3284,27 @@
         <v>9</v>
       </c>
       <c r="G4" s="21">
-        <f>COUNTIF($L$11:$L$595,"PASSED")/COUNTA($L$11:$L$595)</f>
+        <f>COUNTIF($L$11:$L$599,"Pass")</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="21">
+        <f>COUNTIF($N$11:N$599,"Pass")</f>
         <v>1</v>
       </c>
-      <c r="N4" s="21">
-        <f>COUNTIF($N$11:N$595,"Pass")</f>
+      <c r="O4" s="21">
+        <f>COUNTIF($O$11:O$599,"Pass")</f>
         <v>0</v>
       </c>
-      <c r="O4" s="21">
-        <f>COUNTIF($O$11:O$595,"Pass")</f>
+      <c r="P4" s="21">
+        <f>COUNTIF($P$11:P$599,"Pass")</f>
         <v>0</v>
       </c>
-      <c r="P4" s="21">
-        <f>COUNTIF($P$11:P$595,"Pass")</f>
+      <c r="Q4" s="21">
+        <f>COUNTIF($Q$11:Q$599,"Pass")</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="21">
-        <f>COUNTIF($Q$11:Q$595,"Pass")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" ht="30">
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
@@ -3276,27 +3321,27 @@
         <v>10</v>
       </c>
       <c r="G5" s="21">
-        <f>COUNTIF($L$11:$L$595,"FAILED")/COUNTA($L$11:$L$595)</f>
+        <f>COUNTIF($L$11:$L$599,"Fail")</f>
         <v>0</v>
       </c>
       <c r="N5" s="21">
-        <f>COUNTIF($N$11:N$595,"Fail")</f>
+        <f>COUNTIF($N$11:N$599,"Fail")</f>
         <v>0</v>
       </c>
       <c r="O5" s="21">
-        <f>COUNTIF($O$11:$O$595,"Fail")</f>
+        <f>COUNTIF($O$11:$O$599,"Fail")</f>
+        <v>1</v>
+      </c>
+      <c r="P5" s="21">
+        <f>COUNTIF($P$11:$P$599,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="P5" s="21">
-        <f>COUNTIF($P$11:$P$595,"Fail")</f>
+      <c r="Q5" s="21">
+        <f>COUNTIF($Q$11:$Q$599,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="21">
-        <f>COUNTIF($Q$11:$Q$595,"Fail")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" s="2" customFormat="1" ht="60">
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="16" t="s">
         <v>17</v>
       </c>
@@ -3304,35 +3349,34 @@
         <v>21</v>
       </c>
       <c r="D6" s="21">
-        <f>COUNTIF($G$11:$G$595,"Yes")/COUNTA($A$11:$A$595)</f>
+        <f>COUNTIF($G$11:$G$599,"Yes")/COUNTA($A$11:$A$599)</f>
         <v>1</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="21">
-        <f>COUNTIF($L$12:$L$595,"Not Test")/COUNTA($L$11:$L$595)</f>
+        <f>COUNTIF($L$13:$L$599,"Not Test")</f>
         <v>0</v>
       </c>
       <c r="N6" s="21">
-        <f>COUNTIF($N$11:N$595,"Not Test")</f>
+        <f>COUNTIF($N$11:N$599,"Not Test")</f>
         <v>0</v>
       </c>
       <c r="O6" s="21">
-        <f>COUNTIF($H$11:$H$595,"Not Test")</f>
+        <f>COUNTIF($H$12:$H$600,"Not Test")</f>
         <v>0</v>
       </c>
       <c r="P6" s="21">
-        <f>COUNTIF($P$11:$P$595,"Not Test")</f>
-        <v>0</v>
+        <f>COUNTIF($P$11:$P$599,"Not Test")</f>
+        <v>1</v>
       </c>
       <c r="Q6" s="21">
-        <f>COUNTIF($Q$11:$Q$595,"Not Test")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" s="2" customFormat="1"/>
-    <row r="8" spans="1:20" s="2" customFormat="1">
+        <f>COUNTIF($Q$11:$Q$599,"Not Test")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="G8" s="36" t="s">
         <v>40</v>
       </c>
@@ -3348,9 +3392,8 @@
       <c r="O8" s="37"/>
       <c r="P8" s="37"/>
       <c r="Q8" s="37"/>
-      <c r="T8" s="24"/>
-    </row>
-    <row r="9" spans="1:20" s="2" customFormat="1" ht="60">
+    </row>
+    <row r="9" spans="1:19" ht="30">
       <c r="A9" s="16" t="s">
         <v>0</v>
       </c>
@@ -3408,11 +3451,10 @@
       <c r="S9" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="T9" s="24"/>
-    </row>
-    <row r="10" spans="1:20" s="2" customFormat="1">
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="17" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -3432,509 +3474,36 @@
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
-      <c r="T10" s="24"/>
-    </row>
-    <row r="11" spans="1:20" s="2" customFormat="1" ht="240">
-      <c r="A11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>91</v>
+    </row>
+    <row r="11" spans="1:19" ht="105">
+      <c r="A11" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>129</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="L11" t="s">
-        <v>153</v>
-      </c>
-      <c r="M11" t="s">
-        <v>7</v>
-      </c>
-      <c r="T11" s="24"/>
-    </row>
-    <row r="12" spans="1:20" ht="75">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="L12" t="s">
-        <v>153</v>
-      </c>
-      <c r="M12" t="s">
-        <v>7</v>
-      </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="23"/>
-      <c r="L13" t="s">
-        <v>153</v>
-      </c>
-      <c r="M13" t="s">
-        <v>7</v>
-      </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-    </row>
-    <row r="17" spans="8:10">
-      <c r="H17" s="26"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="26"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="J11" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Config!$E$3:$E$185</xm:f>
-          </x14:formula1>
-          <xm:sqref>I11:I17</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S24"/>
-  <sheetViews>
-    <sheetView topLeftCell="G20" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" width="19" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.85546875" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5703125" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="9" max="9" width="25.42578125" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="10" max="10" width="25.7109375" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="11" max="11" width="19.42578125" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="12" max="12" width="14.85546875" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="13" max="13" width="13.5703125" style="2" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="14" max="17" width="13.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="20" max="16384" width="9.140625" style="2" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="18" customFormat="1">
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="R1" s="20"/>
-    </row>
-    <row r="2" spans="1:19" s="18" customFormat="1">
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="R2" s="20"/>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="21">
-        <f>COUNTIF($L$11:$L$599,"Pass")</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="21">
-        <f>COUNTIF($N$11:N$599,"Pass")</f>
-        <v>1</v>
-      </c>
-      <c r="O4" s="21">
-        <f>COUNTIF($O$11:O$599,"Pass")</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="21">
-        <f>COUNTIF($P$11:P$599,"Pass")</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="21">
-        <f>COUNTIF($Q$11:Q$599,"Pass")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="21">
-        <f>COUNTIF($L$11:$L$599,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="21">
-        <f>COUNTIF($N$11:N$599,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="21">
-        <f>COUNTIF($O$11:$O$599,"Fail")</f>
-        <v>1</v>
-      </c>
-      <c r="P5" s="21">
-        <f>COUNTIF($P$11:$P$599,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="21">
-        <f>COUNTIF($Q$11:$Q$599,"Fail")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="21">
-        <f>COUNTIF($G$11:$G$599,"Yes")/COUNTA($A$11:$A$599)</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="21">
-        <f>COUNTIF($L$13:$L$599,"Not Test")</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="21">
-        <f>COUNTIF($N$11:N$599,"Not Test")</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="21">
-        <f>COUNTIF($H$11:$H$599,"Not Test")</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="21">
-        <f>COUNTIF($P$11:$P$599,"Not Test")</f>
-        <v>1</v>
-      </c>
-      <c r="Q6" s="21">
-        <f>COUNTIF($Q$11:$Q$599,"Not Test")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="G8" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-    </row>
-    <row r="9" spans="1:19" ht="30">
-      <c r="A9" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q9" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-    </row>
-    <row r="11" spans="1:19" ht="105">
-      <c r="A11" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" t="s">
-        <v>153</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="L11"/>
       <c r="M11" t="s">
         <v>7</v>
       </c>
@@ -3963,21 +3532,16 @@
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
-      <c r="H12" s="4" t="s">
-        <v>84</v>
+      <c r="H12" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K12" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="L12" t="s">
-        <v>153</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="L12"/>
       <c r="M12" t="s">
         <v>7</v>
       </c>
@@ -3985,96 +3549,89 @@
     </row>
     <row r="13" spans="1:19">
       <c r="H13" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>55</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="L13" t="s">
-        <v>153</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13"/>
       <c r="M13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="H14" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K14" s="4"/>
-      <c r="L14" t="s">
-        <v>153</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14"/>
       <c r="M14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="H15" s="2" t="s">
-        <v>114</v>
+      <c r="H15" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="L15" t="s">
-        <v>153</v>
-      </c>
+      <c r="J15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15"/>
       <c r="M15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="30">
+    <row r="16" spans="1:19">
       <c r="H16" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>59</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="L16" t="s">
-        <v>153</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="L16"/>
       <c r="M16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="8:13">
+    <row r="17" spans="8:13" ht="30">
       <c r="H17" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>59</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="L17" t="s">
-        <v>153</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="L17"/>
       <c r="M17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="8:13" ht="30">
+    <row r="18" spans="8:13">
       <c r="H18" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>59</v>
@@ -4082,118 +3639,131 @@
       <c r="J18" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="L18" t="s">
-        <v>153</v>
-      </c>
+      <c r="L18"/>
       <c r="M18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="8:13">
+    <row r="19" spans="8:13" ht="30">
       <c r="H19" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L19" t="s">
-        <v>153</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="L19"/>
       <c r="M19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="8:13">
       <c r="H20" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>55</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="L20" t="s">
-        <v>153</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="L20"/>
       <c r="M20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="8:13" ht="30">
+    <row r="21" spans="8:13">
       <c r="H21" s="2" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="I21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L21"/>
+      <c r="M21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="8:13" ht="30">
+      <c r="H22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L21" t="s">
-        <v>153</v>
-      </c>
-      <c r="M21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="8:13">
-      <c r="H22" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="L22" t="s">
-        <v>153</v>
-      </c>
+      <c r="J22" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L22"/>
       <c r="M22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="8:13">
       <c r="H23" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K23" s="2">
-        <v>3</v>
-      </c>
-      <c r="L23" t="s">
-        <v>153</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L23"/>
       <c r="M23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="8:13">
       <c r="H24" s="2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="L24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K24" s="2">
+        <v>3</v>
+      </c>
+      <c r="L24"/>
+      <c r="M24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="8:13">
+      <c r="H25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L25"/>
+      <c r="M25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="8:13">
+      <c r="H26" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="M24" t="s">
+      <c r="I26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26"/>
+      <c r="M26" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4266,8 +3836,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="J11" r:id="rId1"/>
-    <hyperlink ref="K13" r:id="rId2"/>
+    <hyperlink ref="J12" r:id="rId1"/>
+    <hyperlink ref="K14" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4276,9 +3846,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Config!$E$3:$E$185</xm:f>
+            <xm:f>Config!$E$3:$E$187</xm:f>
           </x14:formula1>
-          <xm:sqref>I11:I27</xm:sqref>
+          <xm:sqref>I11:I28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>